<commit_message>
Added laboratory and fumehood class
</commit_message>
<xml_diff>
--- a/LifeSciences.xlsx
+++ b/LifeSciences.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="4" r:id="rId1"/>
@@ -63,18 +63,12 @@
     <t>ceil_height</t>
   </si>
   <si>
-    <t>hoods</t>
-  </si>
-  <si>
     <t>Area (sqft)</t>
   </si>
   <si>
     <t>Ceiling (ft)</t>
   </si>
   <si>
-    <t>Hood List</t>
-  </si>
-  <si>
     <t>Lab Name</t>
   </si>
   <si>
@@ -697,6 +691,12 @@
   </si>
   <si>
     <t>as_is</t>
+  </si>
+  <si>
+    <t>num_hoods</t>
+  </si>
+  <si>
+    <t>Number of Hoods</t>
   </si>
 </sst>
 </file>
@@ -1177,29 +1177,29 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" ht="16.05" customHeight="1">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" ht="16.05" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.05" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" s="1">
         <v>26</v>
@@ -1222,11 +1222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="W10" sqref="W10"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.05" customHeight="1"/>
@@ -1240,13 +1240,13 @@
   <sheetData>
     <row r="1" spans="1:23" ht="16.05" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
@@ -1258,7 +1258,7 @@
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
       <c r="O1" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P1" s="9"/>
       <c r="Q1" s="9"/>
@@ -1268,83 +1268,83 @@
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
       <c r="W1" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="2" customFormat="1" ht="16.05" customHeight="1">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" s="6" t="s">
-        <v>5</v>
+        <v>213</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>105</v>
-      </c>
       <c r="W2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="16.05" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -1353,69 +1353,69 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>2</v>
+        <v>212</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="O3" s="1" t="s">
+      <c r="R3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="W3" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="16.05" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>1330.6333179999999</v>
@@ -1477,7 +1477,7 @@
     </row>
     <row r="5" spans="1:23" ht="16.05" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>1305.7687089999999</v>
@@ -1539,7 +1539,7 @@
     </row>
     <row r="6" spans="1:23" ht="16.05" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>1320.73053</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="7" spans="1:23" ht="16.05" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>1312.9805220000001</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="8" spans="1:23" ht="16.05" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>1325.681924</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="9" spans="1:23" ht="16.05" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>1306.629821</v>
@@ -1787,7 +1787,7 @@
     </row>
     <row r="10" spans="1:23" ht="16.05" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B10" s="1">
         <v>1315.133302</v>
@@ -1849,7 +1849,7 @@
     </row>
     <row r="11" spans="1:23" ht="16.05" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B11" s="1">
         <v>1312.6576050000001</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="12" spans="1:23" ht="16.05" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B12" s="1">
         <v>1330.2027619999999</v>
@@ -1973,7 +1973,7 @@
     </row>
     <row r="13" spans="1:23" ht="16.05" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1">
         <v>122.385543</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="14" spans="1:23" ht="16.05" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="1">
         <v>1305.7687089999999</v>
@@ -2097,7 +2097,7 @@
     </row>
     <row r="15" spans="1:23" ht="16.05" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1">
         <v>1315.133302</v>
@@ -2159,7 +2159,7 @@
     </row>
     <row r="16" spans="1:23" ht="16.05" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B16" s="1">
         <v>1312.7652439999999</v>
@@ -2221,7 +2221,7 @@
     </row>
     <row r="17" spans="1:23" ht="16.05" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B17" s="1">
         <v>1330.2027619999999</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="18" spans="1:23" ht="16.05" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1">
         <v>1305.7687089999999</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="19" spans="1:23" ht="16.05" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B19" s="1">
         <v>1315.133302</v>
@@ -2407,7 +2407,7 @@
     </row>
     <row r="20" spans="1:23" ht="16.05" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B20" s="1">
         <v>1312.6576050000001</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="21" spans="1:23" ht="16.05" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B21" s="1">
         <v>433.13933600000001</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="22" spans="1:23" ht="16.05" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B22" s="1">
         <v>338.09409900000003</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="23" spans="1:23" ht="16.05" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B23" s="1">
         <v>548.420705</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="24" spans="1:23" ht="16.05" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="1">
         <v>359.62189899999998</v>
@@ -2717,7 +2717,7 @@
     </row>
     <row r="25" spans="1:23" ht="16.05" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="1">
         <v>600</v>
@@ -2777,12 +2777,12 @@
         <v>0.1</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="16.05" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B26" s="1">
         <v>500.41371099999998</v>
@@ -2844,7 +2844,7 @@
     </row>
     <row r="27" spans="1:23" ht="16.05" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B27" s="1">
         <v>613.54229999999995</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="28" spans="1:23" ht="16.05" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B28" s="1">
         <v>1735.3559580000001</v>
@@ -2968,7 +2968,7 @@
     </row>
     <row r="29" spans="1:23" ht="16.05" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1">
         <v>111.40636499999999</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="30" spans="1:23" ht="16.05" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1">
         <v>1902.626964</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="31" spans="1:23" ht="16.05" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" s="1">
         <v>1679.921873</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="32" spans="1:23" ht="16.05" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B32" s="1">
         <v>79.329943</v>
@@ -3216,7 +3216,7 @@
     </row>
     <row r="33" spans="1:22" ht="16.05" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" s="1">
         <v>1901.9811299999999</v>
@@ -3278,7 +3278,7 @@
     </row>
     <row r="34" spans="1:22" ht="16.05" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B34" s="1">
         <v>1682.182292</v>
@@ -3340,7 +3340,7 @@
     </row>
     <row r="35" spans="1:22" ht="16.05" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B35" s="1">
         <v>115.281369</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="36" spans="1:22" ht="16.05" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1">
         <v>118.079983</v>
@@ -3488,7 +3488,7 @@
   <dimension ref="A1:K169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
@@ -3503,101 +3503,101 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.05" customHeight="1">
       <c r="A1" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
       <c r="I1" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J1" s="9"/>
       <c r="K1" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="16.05" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>194</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16.05" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="H3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>18</v>
-      </c>
       <c r="I3" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16.05" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8">
         <v>29.5</v>
@@ -3618,7 +3618,7 @@
         <v>100</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J4" s="8">
         <v>0.4</v>
@@ -3627,10 +3627,10 @@
     </row>
     <row r="5" spans="1:11" ht="16.05" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="8">
         <v>29.5</v>
@@ -3651,7 +3651,7 @@
         <v>100</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J5" s="8">
         <v>0.4</v>
@@ -3660,10 +3660,10 @@
     </row>
     <row r="6" spans="1:11" ht="16.05" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" s="8">
         <v>29.5</v>
@@ -3684,7 +3684,7 @@
         <v>100</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J6" s="8">
         <v>0.4</v>
@@ -3693,10 +3693,10 @@
     </row>
     <row r="7" spans="1:11" ht="16.05" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" s="8">
         <v>29.5</v>
@@ -3717,7 +3717,7 @@
         <v>100</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J7" s="8">
         <v>0.4</v>
@@ -3726,10 +3726,10 @@
     </row>
     <row r="8" spans="1:11" ht="16.05" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C8" s="8">
         <v>29.5</v>
@@ -3750,7 +3750,7 @@
         <v>100</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J8" s="8">
         <v>0.4</v>
@@ -3759,10 +3759,10 @@
     </row>
     <row r="9" spans="1:11" ht="16.05" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="8">
         <v>29.5</v>
@@ -3783,7 +3783,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J9" s="8">
         <v>0.4</v>
@@ -3792,10 +3792,10 @@
     </row>
     <row r="10" spans="1:11" ht="16.05" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="8">
         <v>29.5</v>
@@ -3816,7 +3816,7 @@
         <v>100</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J10" s="8">
         <v>0.4</v>
@@ -3825,10 +3825,10 @@
     </row>
     <row r="11" spans="1:11" ht="16.05" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C11" s="8">
         <v>29.5</v>
@@ -3849,7 +3849,7 @@
         <v>100</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J11" s="8">
         <v>0.4</v>
@@ -3858,10 +3858,10 @@
     </row>
     <row r="12" spans="1:11" ht="16.05" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="8">
         <v>29.5</v>
@@ -3882,7 +3882,7 @@
         <v>100</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J12" s="8">
         <v>0.4</v>
@@ -3891,10 +3891,10 @@
     </row>
     <row r="13" spans="1:11" ht="16.05" customHeight="1">
       <c r="A13" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" s="8">
         <v>29.5</v>
@@ -3915,7 +3915,7 @@
         <v>100</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J13" s="8">
         <v>0.4</v>
@@ -3924,10 +3924,10 @@
     </row>
     <row r="14" spans="1:11" ht="16.05" customHeight="1">
       <c r="A14" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="8">
         <v>29.5</v>
@@ -3948,7 +3948,7 @@
         <v>100</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J14" s="8">
         <v>0.4</v>
@@ -3957,10 +3957,10 @@
     </row>
     <row r="15" spans="1:11" ht="16.05" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C15" s="8">
         <v>29.5</v>
@@ -3981,7 +3981,7 @@
         <v>100</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J15" s="8">
         <v>0.4</v>
@@ -3990,10 +3990,10 @@
     </row>
     <row r="16" spans="1:11" ht="16.05" customHeight="1">
       <c r="A16" s="8" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C16" s="8">
         <v>29.5</v>
@@ -4014,7 +4014,7 @@
         <v>100</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J16" s="8">
         <v>0.4</v>
@@ -4023,10 +4023,10 @@
     </row>
     <row r="17" spans="1:11" ht="16.05" customHeight="1">
       <c r="A17" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="8">
         <v>29.5</v>
@@ -4047,7 +4047,7 @@
         <v>100</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J17" s="8">
         <v>0.4</v>
@@ -4056,10 +4056,10 @@
     </row>
     <row r="18" spans="1:11" ht="16.05" customHeight="1">
       <c r="A18" s="8" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C18" s="8">
         <v>29.5</v>
@@ -4080,7 +4080,7 @@
         <v>100</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J18" s="8">
         <v>0.4</v>
@@ -4089,10 +4089,10 @@
     </row>
     <row r="19" spans="1:11" ht="16.05" customHeight="1">
       <c r="A19" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="8">
         <v>29.5</v>
@@ -4113,7 +4113,7 @@
         <v>100</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J19" s="8">
         <v>0.4</v>
@@ -4122,10 +4122,10 @@
     </row>
     <row r="20" spans="1:11" ht="16.05" customHeight="1">
       <c r="A20" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="8">
         <v>29.5</v>
@@ -4146,7 +4146,7 @@
         <v>100</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J20" s="8">
         <v>0.4</v>
@@ -4155,10 +4155,10 @@
     </row>
     <row r="21" spans="1:11" ht="16.05" customHeight="1">
       <c r="A21" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C21" s="8">
         <v>29.5</v>
@@ -4179,7 +4179,7 @@
         <v>100</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J21" s="8">
         <v>0.4</v>
@@ -4188,10 +4188,10 @@
     </row>
     <row r="22" spans="1:11" ht="16.05" customHeight="1">
       <c r="A22" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C22" s="8">
         <v>29.5</v>
@@ -4212,7 +4212,7 @@
         <v>100</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J22" s="8">
         <v>0.4</v>
@@ -4221,10 +4221,10 @@
     </row>
     <row r="23" spans="1:11" ht="16.05" customHeight="1">
       <c r="A23" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C23" s="8">
         <v>29.5</v>
@@ -4245,7 +4245,7 @@
         <v>100</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J23" s="8">
         <v>0.4</v>
@@ -4254,10 +4254,10 @@
     </row>
     <row r="24" spans="1:11" ht="16.05" customHeight="1">
       <c r="A24" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C24" s="8">
         <v>29.5</v>
@@ -4278,7 +4278,7 @@
         <v>100</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J24" s="8">
         <v>0.4</v>
@@ -4287,10 +4287,10 @@
     </row>
     <row r="25" spans="1:11" ht="16.05" customHeight="1">
       <c r="A25" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C25" s="8">
         <v>29.5</v>
@@ -4311,7 +4311,7 @@
         <v>100</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J25" s="8">
         <v>0.4</v>
@@ -4320,10 +4320,10 @@
     </row>
     <row r="26" spans="1:11" ht="16.05" customHeight="1">
       <c r="A26" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C26" s="8">
         <v>29.5</v>
@@ -4344,7 +4344,7 @@
         <v>100</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J26" s="8">
         <v>0.4</v>
@@ -4353,10 +4353,10 @@
     </row>
     <row r="27" spans="1:11" ht="16.05" customHeight="1">
       <c r="A27" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C27" s="8">
         <v>29.5</v>
@@ -4377,7 +4377,7 @@
         <v>100</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J27" s="8">
         <v>0.4</v>
@@ -4386,10 +4386,10 @@
     </row>
     <row r="28" spans="1:11" ht="16.05" customHeight="1">
       <c r="A28" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C28" s="8">
         <v>29.5</v>
@@ -4410,7 +4410,7 @@
         <v>100</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J28" s="8">
         <v>0.4</v>
@@ -4419,10 +4419,10 @@
     </row>
     <row r="29" spans="1:11" ht="16.05" customHeight="1">
       <c r="A29" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C29" s="8">
         <v>29.5</v>
@@ -4443,7 +4443,7 @@
         <v>100</v>
       </c>
       <c r="I29" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J29" s="8">
         <v>0.4</v>
@@ -4452,10 +4452,10 @@
     </row>
     <row r="30" spans="1:11" ht="16.05" customHeight="1">
       <c r="A30" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" s="8">
         <v>29.5</v>
@@ -4476,7 +4476,7 @@
         <v>100</v>
       </c>
       <c r="I30" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J30" s="8">
         <v>0.4</v>
@@ -4485,10 +4485,10 @@
     </row>
     <row r="31" spans="1:11" ht="16.05" customHeight="1">
       <c r="A31" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C31" s="8">
         <v>29.5</v>
@@ -4509,7 +4509,7 @@
         <v>100</v>
       </c>
       <c r="I31" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J31" s="8">
         <v>0.4</v>
@@ -4518,10 +4518,10 @@
     </row>
     <row r="32" spans="1:11" ht="16.05" customHeight="1">
       <c r="A32" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C32" s="8">
         <v>29.5</v>
@@ -4542,7 +4542,7 @@
         <v>100</v>
       </c>
       <c r="I32" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J32" s="8">
         <v>0.4</v>
@@ -4551,10 +4551,10 @@
     </row>
     <row r="33" spans="1:11" ht="16.05" customHeight="1">
       <c r="A33" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" s="8">
         <v>29.5</v>
@@ -4575,7 +4575,7 @@
         <v>100</v>
       </c>
       <c r="I33" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J33" s="8">
         <v>0.4</v>
@@ -4584,10 +4584,10 @@
     </row>
     <row r="34" spans="1:11" ht="16.05" customHeight="1">
       <c r="A34" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" s="8">
         <v>29.5</v>
@@ -4608,7 +4608,7 @@
         <v>100</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J34" s="8">
         <v>0.4</v>
@@ -4617,10 +4617,10 @@
     </row>
     <row r="35" spans="1:11" ht="16.05" customHeight="1">
       <c r="A35" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C35" s="8">
         <v>29.5</v>
@@ -4641,7 +4641,7 @@
         <v>100</v>
       </c>
       <c r="I35" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J35" s="8">
         <v>0.4</v>
@@ -4650,10 +4650,10 @@
     </row>
     <row r="36" spans="1:11" ht="16.05" customHeight="1">
       <c r="A36" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C36" s="8">
         <v>29.5</v>
@@ -4674,7 +4674,7 @@
         <v>100</v>
       </c>
       <c r="I36" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J36" s="8">
         <v>0.4</v>
@@ -4683,10 +4683,10 @@
     </row>
     <row r="37" spans="1:11" ht="16.05" customHeight="1">
       <c r="A37" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C37" s="8">
         <v>29.5</v>
@@ -4707,7 +4707,7 @@
         <v>100</v>
       </c>
       <c r="I37" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J37" s="8">
         <v>0.4</v>
@@ -4716,10 +4716,10 @@
     </row>
     <row r="38" spans="1:11" ht="16.05" customHeight="1">
       <c r="A38" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C38" s="8">
         <v>29.5</v>
@@ -4740,7 +4740,7 @@
         <v>100</v>
       </c>
       <c r="I38" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J38" s="8">
         <v>0.4</v>
@@ -4749,10 +4749,10 @@
     </row>
     <row r="39" spans="1:11" ht="16.05" customHeight="1">
       <c r="A39" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C39" s="8">
         <v>29.5</v>
@@ -4773,7 +4773,7 @@
         <v>100</v>
       </c>
       <c r="I39" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J39" s="8">
         <v>0.4</v>
@@ -4782,10 +4782,10 @@
     </row>
     <row r="40" spans="1:11" ht="16.05" customHeight="1">
       <c r="A40" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C40" s="8">
         <v>29.5</v>
@@ -4806,7 +4806,7 @@
         <v>100</v>
       </c>
       <c r="I40" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J40" s="8">
         <v>0.4</v>
@@ -4815,10 +4815,10 @@
     </row>
     <row r="41" spans="1:11" ht="16.05" customHeight="1">
       <c r="A41" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C41" s="8">
         <v>29.5</v>
@@ -4839,7 +4839,7 @@
         <v>100</v>
       </c>
       <c r="I41" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J41" s="8">
         <v>0.4</v>
@@ -4848,10 +4848,10 @@
     </row>
     <row r="42" spans="1:11" ht="16.05" customHeight="1">
       <c r="A42" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C42" s="8">
         <v>29.5</v>
@@ -4872,7 +4872,7 @@
         <v>100</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J42" s="8">
         <v>0.4</v>
@@ -4881,10 +4881,10 @@
     </row>
     <row r="43" spans="1:11" ht="16.05" customHeight="1">
       <c r="A43" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C43" s="8">
         <v>29.5</v>
@@ -4905,7 +4905,7 @@
         <v>100</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J43" s="8">
         <v>0.4</v>
@@ -4914,10 +4914,10 @@
     </row>
     <row r="44" spans="1:11" ht="16.05" customHeight="1">
       <c r="A44" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C44" s="8">
         <v>29.5</v>
@@ -4938,7 +4938,7 @@
         <v>100</v>
       </c>
       <c r="I44" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J44" s="8">
         <v>0.4</v>
@@ -4947,10 +4947,10 @@
     </row>
     <row r="45" spans="1:11" ht="16.05" customHeight="1">
       <c r="A45" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C45" s="8">
         <v>29.5</v>
@@ -4971,7 +4971,7 @@
         <v>100</v>
       </c>
       <c r="I45" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J45" s="8">
         <v>0.4</v>
@@ -4980,10 +4980,10 @@
     </row>
     <row r="46" spans="1:11" ht="16.05" customHeight="1">
       <c r="A46" s="8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C46" s="8">
         <v>29.5</v>
@@ -5004,7 +5004,7 @@
         <v>100</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J46" s="8">
         <v>0.4</v>
@@ -5013,10 +5013,10 @@
     </row>
     <row r="47" spans="1:11" ht="16.05" customHeight="1">
       <c r="A47" s="8" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C47" s="8">
         <v>29.5</v>
@@ -5037,7 +5037,7 @@
         <v>100</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J47" s="8">
         <v>0.4</v>
@@ -5046,10 +5046,10 @@
     </row>
     <row r="48" spans="1:11" ht="16.05" customHeight="1">
       <c r="A48" s="8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C48" s="8">
         <v>29.5</v>
@@ -5070,7 +5070,7 @@
         <v>100</v>
       </c>
       <c r="I48" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J48" s="8">
         <v>0.4</v>
@@ -5079,10 +5079,10 @@
     </row>
     <row r="49" spans="1:11" ht="16.05" customHeight="1">
       <c r="A49" s="8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C49" s="8">
         <v>29.5</v>
@@ -5103,7 +5103,7 @@
         <v>100</v>
       </c>
       <c r="I49" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J49" s="8">
         <v>0.4</v>
@@ -5112,10 +5112,10 @@
     </row>
     <row r="50" spans="1:11" ht="16.05" customHeight="1">
       <c r="A50" s="8" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C50" s="8">
         <v>29.5</v>
@@ -5136,7 +5136,7 @@
         <v>100</v>
       </c>
       <c r="I50" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J50" s="8">
         <v>0.4</v>
@@ -5145,10 +5145,10 @@
     </row>
     <row r="51" spans="1:11" ht="16.05" customHeight="1">
       <c r="A51" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C51" s="8">
         <v>29.5</v>
@@ -5169,7 +5169,7 @@
         <v>100</v>
       </c>
       <c r="I51" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J51" s="8">
         <v>0.4</v>
@@ -5178,10 +5178,10 @@
     </row>
     <row r="52" spans="1:11" ht="16.05" customHeight="1">
       <c r="A52" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C52" s="8">
         <v>29.5</v>
@@ -5202,7 +5202,7 @@
         <v>100</v>
       </c>
       <c r="I52" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J52" s="8">
         <v>0.4</v>
@@ -5211,10 +5211,10 @@
     </row>
     <row r="53" spans="1:11" ht="16.05" customHeight="1">
       <c r="A53" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C53" s="8">
         <v>29.5</v>
@@ -5235,7 +5235,7 @@
         <v>100</v>
       </c>
       <c r="I53" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J53" s="8">
         <v>0.4</v>
@@ -5244,10 +5244,10 @@
     </row>
     <row r="54" spans="1:11" ht="16.05" customHeight="1">
       <c r="A54" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C54" s="8">
         <v>29.5</v>
@@ -5268,7 +5268,7 @@
         <v>100</v>
       </c>
       <c r="I54" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J54" s="8">
         <v>0.4</v>
@@ -5277,10 +5277,10 @@
     </row>
     <row r="55" spans="1:11" ht="16.05" customHeight="1">
       <c r="A55" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C55" s="8">
         <v>29.5</v>
@@ -5301,7 +5301,7 @@
         <v>100</v>
       </c>
       <c r="I55" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J55" s="8">
         <v>0.4</v>
@@ -5310,10 +5310,10 @@
     </row>
     <row r="56" spans="1:11" ht="16.05" customHeight="1">
       <c r="A56" s="8" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C56" s="8">
         <v>29.5</v>
@@ -5334,7 +5334,7 @@
         <v>100</v>
       </c>
       <c r="I56" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J56" s="8">
         <v>0.4</v>
@@ -5343,10 +5343,10 @@
     </row>
     <row r="57" spans="1:11" ht="16.05" customHeight="1">
       <c r="A57" s="8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C57" s="8">
         <v>29.5</v>
@@ -5367,7 +5367,7 @@
         <v>100</v>
       </c>
       <c r="I57" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J57" s="8">
         <v>0.4</v>
@@ -5376,10 +5376,10 @@
     </row>
     <row r="58" spans="1:11" ht="16.05" customHeight="1">
       <c r="A58" s="8" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C58" s="8">
         <v>29.5</v>
@@ -5400,7 +5400,7 @@
         <v>100</v>
       </c>
       <c r="I58" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J58" s="8">
         <v>0.4</v>
@@ -5409,10 +5409,10 @@
     </row>
     <row r="59" spans="1:11" ht="16.05" customHeight="1">
       <c r="A59" s="8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C59" s="8">
         <v>29.5</v>
@@ -5433,7 +5433,7 @@
         <v>100</v>
       </c>
       <c r="I59" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J59" s="8">
         <v>0.4</v>
@@ -5442,10 +5442,10 @@
     </row>
     <row r="60" spans="1:11" ht="16.05" customHeight="1">
       <c r="A60" s="8" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C60" s="8">
         <v>29.5</v>
@@ -5466,7 +5466,7 @@
         <v>100</v>
       </c>
       <c r="I60" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J60" s="8">
         <v>0.4</v>
@@ -5475,10 +5475,10 @@
     </row>
     <row r="61" spans="1:11" ht="16.05" customHeight="1">
       <c r="A61" s="8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C61" s="8">
         <v>29.5</v>
@@ -5499,7 +5499,7 @@
         <v>100</v>
       </c>
       <c r="I61" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J61" s="8">
         <v>0.4</v>
@@ -5508,10 +5508,10 @@
     </row>
     <row r="62" spans="1:11" ht="16.05" customHeight="1">
       <c r="A62" s="8" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C62" s="8">
         <v>29.5</v>
@@ -5532,7 +5532,7 @@
         <v>100</v>
       </c>
       <c r="I62" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J62" s="8">
         <v>0.4</v>
@@ -5541,10 +5541,10 @@
     </row>
     <row r="63" spans="1:11" ht="16.05" customHeight="1">
       <c r="A63" s="8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C63" s="8">
         <v>29.5</v>
@@ -5565,7 +5565,7 @@
         <v>100</v>
       </c>
       <c r="I63" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J63" s="8">
         <v>0.4</v>
@@ -5574,10 +5574,10 @@
     </row>
     <row r="64" spans="1:11" ht="16.05" customHeight="1">
       <c r="A64" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C64" s="8">
         <v>29.5</v>
@@ -5598,7 +5598,7 @@
         <v>100</v>
       </c>
       <c r="I64" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J64" s="8">
         <v>0.4</v>
@@ -5607,10 +5607,10 @@
     </row>
     <row r="65" spans="1:11" ht="16.05" customHeight="1">
       <c r="A65" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C65" s="8">
         <v>29.5</v>
@@ -5631,7 +5631,7 @@
         <v>100</v>
       </c>
       <c r="I65" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J65" s="8">
         <v>0.4</v>
@@ -5640,10 +5640,10 @@
     </row>
     <row r="66" spans="1:11" ht="16.05" customHeight="1">
       <c r="A66" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C66" s="8">
         <v>29.5</v>
@@ -5664,7 +5664,7 @@
         <v>100</v>
       </c>
       <c r="I66" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J66" s="8">
         <v>0.4</v>
@@ -5673,10 +5673,10 @@
     </row>
     <row r="67" spans="1:11" ht="16.05" customHeight="1">
       <c r="A67" s="8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C67" s="8">
         <v>29.5</v>
@@ -5697,7 +5697,7 @@
         <v>100</v>
       </c>
       <c r="I67" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J67" s="8">
         <v>0.4</v>
@@ -7055,11 +7055,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="16.05" customHeight="1"/>
@@ -7069,128 +7069,128 @@
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="16.05" customHeight="1">
       <c r="A1" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.05" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.05" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.05" customHeight="1">
       <c r="A4" s="8" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.05" customHeight="1">
       <c r="A5" s="8" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.05" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.05" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.05" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.05" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>211</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final changes before McGill Sim
</commit_message>
<xml_diff>
--- a/LifeSciences.xlsx
+++ b/LifeSciences.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="4" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="218">
   <si>
     <t>surface_area</t>
   </si>
@@ -706,6 +706,9 @@
   </si>
   <si>
     <t>worst_case_usage</t>
+  </si>
+  <si>
+    <t>PIR</t>
   </si>
 </sst>
 </file>
@@ -800,7 +803,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1214,7 +1224,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1227,11 +1237,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AP36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="L4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="V3" sqref="V3"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.05" customHeight="1"/>
@@ -1455,6 +1465,9 @@
       <c r="M4" s="1">
         <v>0</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O4" s="1">
         <v>0.9</v>
       </c>
@@ -1517,6 +1530,9 @@
       <c r="M5" s="1">
         <v>0</v>
       </c>
+      <c r="N5" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O5" s="1">
         <v>0.9</v>
       </c>
@@ -1579,6 +1595,9 @@
       <c r="M6" s="1">
         <v>0</v>
       </c>
+      <c r="N6" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O6" s="1">
         <v>0.9</v>
       </c>
@@ -1641,6 +1660,9 @@
       <c r="M7" s="1">
         <v>0</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O7" s="1">
         <v>0.9</v>
       </c>
@@ -1703,6 +1725,9 @@
       <c r="M8" s="1">
         <v>0</v>
       </c>
+      <c r="N8" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O8" s="1">
         <v>0.9</v>
       </c>
@@ -1765,6 +1790,9 @@
       <c r="M9" s="1">
         <v>0</v>
       </c>
+      <c r="N9" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O9" s="1">
         <v>0.9</v>
       </c>
@@ -1827,6 +1855,9 @@
       <c r="M10" s="1">
         <v>0</v>
       </c>
+      <c r="N10" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O10" s="1">
         <v>0.9</v>
       </c>
@@ -1889,6 +1920,9 @@
       <c r="M11" s="1">
         <v>0</v>
       </c>
+      <c r="N11" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O11" s="1">
         <v>0.9</v>
       </c>
@@ -1951,6 +1985,9 @@
       <c r="M12" s="1">
         <v>0</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O12" s="1">
         <v>0.9</v>
       </c>
@@ -2013,6 +2050,9 @@
       <c r="M13" s="1">
         <v>0</v>
       </c>
+      <c r="N13" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O13" s="1">
         <v>0.9</v>
       </c>
@@ -2075,6 +2115,9 @@
       <c r="M14" s="1">
         <v>0</v>
       </c>
+      <c r="N14" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O14" s="1">
         <v>0.9</v>
       </c>
@@ -2137,6 +2180,9 @@
       <c r="M15" s="1">
         <v>0</v>
       </c>
+      <c r="N15" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O15" s="1">
         <v>0.9</v>
       </c>
@@ -2199,6 +2245,9 @@
       <c r="M16" s="1">
         <v>0</v>
       </c>
+      <c r="N16" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O16" s="1">
         <v>0.9</v>
       </c>
@@ -2261,6 +2310,9 @@
       <c r="M17" s="1">
         <v>0</v>
       </c>
+      <c r="N17" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O17" s="1">
         <v>0.9</v>
       </c>
@@ -2323,6 +2375,9 @@
       <c r="M18" s="1">
         <v>0</v>
       </c>
+      <c r="N18" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O18" s="1">
         <v>0.9</v>
       </c>
@@ -2385,6 +2440,9 @@
       <c r="M19" s="1">
         <v>0</v>
       </c>
+      <c r="N19" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O19" s="1">
         <v>0.9</v>
       </c>
@@ -2447,6 +2505,9 @@
       <c r="M20" s="1">
         <v>0</v>
       </c>
+      <c r="N20" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O20" s="1">
         <v>0.9</v>
       </c>
@@ -2509,6 +2570,9 @@
       <c r="M21" s="1">
         <v>0</v>
       </c>
+      <c r="N21" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O21" s="1">
         <v>0.9</v>
       </c>
@@ -2571,6 +2635,9 @@
       <c r="M22" s="1">
         <v>0</v>
       </c>
+      <c r="N22" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O22" s="1">
         <v>0.9</v>
       </c>
@@ -2633,6 +2700,9 @@
       <c r="M23" s="1">
         <v>0</v>
       </c>
+      <c r="N23" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O23" s="1">
         <v>0.9</v>
       </c>
@@ -2695,6 +2765,9 @@
       <c r="M24" s="1">
         <v>0</v>
       </c>
+      <c r="N24" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O24" s="1">
         <v>0.9</v>
       </c>
@@ -2757,6 +2830,9 @@
       <c r="M25" s="1">
         <v>0</v>
       </c>
+      <c r="N25" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O25" s="1">
         <v>0.9</v>
       </c>
@@ -2822,6 +2898,9 @@
       <c r="M26" s="1">
         <v>0</v>
       </c>
+      <c r="N26" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O26" s="1">
         <v>0.9</v>
       </c>
@@ -2884,6 +2963,9 @@
       <c r="M27" s="1">
         <v>0</v>
       </c>
+      <c r="N27" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O27" s="1">
         <v>0.9</v>
       </c>
@@ -2946,6 +3028,9 @@
       <c r="M28" s="1">
         <v>0</v>
       </c>
+      <c r="N28" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O28" s="1">
         <v>0.9</v>
       </c>
@@ -3008,6 +3093,9 @@
       <c r="M29" s="1">
         <v>0</v>
       </c>
+      <c r="N29" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O29" s="1">
         <v>0.9</v>
       </c>
@@ -3070,6 +3158,9 @@
       <c r="M30" s="1">
         <v>0</v>
       </c>
+      <c r="N30" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O30" s="1">
         <v>0.9</v>
       </c>
@@ -3132,6 +3223,9 @@
       <c r="M31" s="1">
         <v>0</v>
       </c>
+      <c r="N31" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O31" s="1">
         <v>0.9</v>
       </c>
@@ -3194,6 +3288,9 @@
       <c r="M32" s="1">
         <v>0</v>
       </c>
+      <c r="N32" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O32" s="1">
         <v>0.9</v>
       </c>
@@ -3256,6 +3353,9 @@
       <c r="M33" s="1">
         <v>0</v>
       </c>
+      <c r="N33" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O33" s="1">
         <v>0.9</v>
       </c>
@@ -3318,6 +3418,9 @@
       <c r="M34" s="1">
         <v>0</v>
       </c>
+      <c r="N34" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O34" s="1">
         <v>0.9</v>
       </c>
@@ -3380,6 +3483,9 @@
       <c r="M35" s="1">
         <v>0</v>
       </c>
+      <c r="N35" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="O35" s="1">
         <v>0.9</v>
       </c>
@@ -3441,6 +3547,9 @@
       </c>
       <c r="M36" s="1">
         <v>0</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>217</v>
       </c>
       <c r="O36" s="1">
         <v>0.9</v>
@@ -3473,13 +3582,13 @@
     <mergeCell ref="E1:N1"/>
     <mergeCell ref="O1:V1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:N1048576 A1:A1048576 E1 O1:O1048576 W1:XFD1048576 P2:V1048576">
-    <cfRule type="expression" dxfId="9" priority="3">
+  <conditionalFormatting sqref="A1:A1048576 E1 O1:O1048576 W1:XFD1048576 P2:V1048576 B2:N1048576">
+    <cfRule type="expression" dxfId="10" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:N1048576 A1:A1048576 E1 O1:O1048576 W1:XFD1048576 P2:V1048576">
-    <cfRule type="expression" dxfId="8" priority="1">
+  <conditionalFormatting sqref="A1:A1048576 E1 O1:O1048576 W1:XFD1048576 P2:V1048576 B2:N1048576">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3492,7 +3601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K169"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -7042,12 +7151,12 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7200,32 +7309,32 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="6" priority="6">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C2">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>